<commit_message>
Updated learners Excel file
</commit_message>
<xml_diff>
--- a/learners.xlsx
+++ b/learners.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4637" uniqueCount="947">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4637" uniqueCount="946">
   <si>
     <t>GENDER</t>
   </si>
@@ -2844,9 +2844,6 @@
   </si>
   <si>
     <t>SIMON GENO</t>
-  </si>
-  <si>
-    <t>BLEESED</t>
   </si>
   <si>
     <t>PRINCE NYLAN</t>
@@ -3348,7 +3345,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M893"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A869" workbookViewId="0">
+      <selection activeCell="F906" sqref="F906"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4522,7 +4521,7 @@
         <v>848</v>
       </c>
       <c r="F39" s="37" t="s">
-        <v>940</v>
+        <v>43</v>
       </c>
       <c r="G39" s="37"/>
       <c r="H39" s="38"/>
@@ -4542,7 +4541,7 @@
       </c>
       <c r="B40" s="37"/>
       <c r="C40" s="37" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="D40" s="37" t="s">
         <v>918</v>
@@ -4571,7 +4570,7 @@
       </c>
       <c r="B41" s="37"/>
       <c r="C41" s="37" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="D41" s="37" t="s">
         <v>918</v>
@@ -4580,7 +4579,7 @@
         <v>848</v>
       </c>
       <c r="F41" s="37" t="s">
-        <v>940</v>
+        <v>43</v>
       </c>
       <c r="G41" s="37"/>
       <c r="H41" s="38"/>
@@ -4631,7 +4630,7 @@
       </c>
       <c r="B43" s="37"/>
       <c r="C43" s="37" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="D43" s="37" t="s">
         <v>918</v>
@@ -4669,7 +4668,7 @@
         <v>848</v>
       </c>
       <c r="F44" s="37" t="s">
-        <v>940</v>
+        <v>43</v>
       </c>
       <c r="G44" s="37"/>
       <c r="H44" s="38"/>
@@ -4731,7 +4730,7 @@
         <v>848</v>
       </c>
       <c r="F46" s="37" t="s">
-        <v>940</v>
+        <v>43</v>
       </c>
       <c r="G46" s="37"/>
       <c r="H46" s="38"/>
@@ -4793,7 +4792,7 @@
         <v>848</v>
       </c>
       <c r="F48" s="37" t="s">
-        <v>940</v>
+        <v>43</v>
       </c>
       <c r="G48" s="37"/>
       <c r="H48" s="38"/>
@@ -4855,7 +4854,7 @@
         <v>848</v>
       </c>
       <c r="F50" s="37" t="s">
-        <v>940</v>
+        <v>43</v>
       </c>
       <c r="G50" s="37"/>
       <c r="H50" s="38"/>
@@ -4904,7 +4903,7 @@
       </c>
       <c r="B52" s="37"/>
       <c r="C52" s="37" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="D52" s="37" t="s">
         <v>918</v>
@@ -5338,7 +5337,7 @@
         <v>14</v>
       </c>
       <c r="C66" s="39" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="D66" s="39" t="s">
         <v>918</v>
@@ -20746,7 +20745,7 @@
       </c>
       <c r="B578" s="35"/>
       <c r="C578" s="35" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="D578" s="35" t="s">
         <v>919</v>

</xml_diff>